<commit_message>
database completo e popolato di tutto
</commit_message>
<xml_diff>
--- a/SoftwareSanitario/database/excel/allDoctors_data.xlsx
+++ b/SoftwareSanitario/database/excel/allDoctors_data.xlsx
@@ -3,14 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="93" documentId="11_AD4D5CB4E552A52AC6156845DA9857005BDEDDA4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{CF56806B-C621-4455-8909-AAEF496C2294}"/>
+  <xr:revisionPtr revIDLastSave="95" documentId="11_AD4D5CB4E552A52AC6156845DA9857005BDEDDA4" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{2E0FE168-1395-48CF-9103-BC972D9C29C2}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="8964" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AllDoctors" sheetId="1" r:id="rId1"/>
-    <sheet name="GeneralDoctors" sheetId="2" r:id="rId2"/>
-    <sheet name="Specialists" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -28,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
   <si>
     <t>Steve</t>
   </si>
@@ -175,15 +173,6 @@
   </si>
   <si>
     <t>linuxhack@me.com</t>
-  </si>
-  <si>
-    <t>Oncology</t>
-  </si>
-  <si>
-    <t>Pediatry</t>
-  </si>
-  <si>
-    <t>Surgery</t>
   </si>
 </sst>
 </file>
@@ -193,7 +182,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd;@"/>
   </numFmts>
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -205,14 +194,6 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -239,7 +220,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -252,7 +233,6 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Collegamento ipertestuale" xfId="1" builtinId="8"/>
@@ -536,7 +516,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G7" sqref="G7:G12"/>
     </sheetView>
   </sheetViews>
@@ -880,115 +860,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1FEA97C5-F6C1-4AB3-AD30-A25B6AF66CB7}">
-  <dimension ref="A1:A6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A1">
-        <v>12345</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>12346</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>12347</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>12348</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>12349</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>12350</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7633C001-87F4-43E6-B553-E9FF02D4D4DE}">
-  <dimension ref="A1:B7"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>49</v>
-      </c>
-      <c r="B1">
-        <v>12351</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>50</v>
-      </c>
-      <c r="B2">
-        <v>12352</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B3">
-        <v>12353</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4">
-        <v>12354</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>12355</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6">
-        <v>12356</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A7" s="6"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>